<commit_message>
OPCN2 Wind Tunnel Test analysis
</commit_message>
<xml_diff>
--- a/Testing/Wind tunnel/Electrostatic sensor 6_Sept.xlsx
+++ b/Testing/Wind tunnel/Electrostatic sensor 6_Sept.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Parth\Documents\uni\FYP\volcanic-ash-uav\Testing\Wind tunnel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jamie\Documents\My Uni Work\3rd Pro\ENMT401\volcanic-ash-uav\Testing\Wind tunnel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -141,7 +141,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -180,7 +180,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -345,6 +344,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FE5A-4982-B402-A64BBEF2BEA6}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -475,6 +479,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FE5A-4982-B402-A64BBEF2BEA6}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -586,7 +595,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -661,7 +669,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -729,7 +736,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -743,7 +750,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -896,6 +902,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6382-45D8-97E8-A6054F361CE5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1014,6 +1025,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6382-45D8-97E8-A6054F361CE5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1132,6 +1148,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6382-45D8-97E8-A6054F361CE5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1250,6 +1271,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-6382-45D8-97E8-A6054F361CE5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1380,7 +1406,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2692,6 +2717,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2727,6 +2769,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -8715,6 +8774,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>